<commit_message>
added fine mapping table
</commit_message>
<xml_diff>
--- a/tables_plots/table_hits_snps_no_covar.xlsx
+++ b/tables_plots/table_hits_snps_no_covar.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,15 +451,20 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>ancestry of the population</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>OR (CI = 95%)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>p value</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>chr</t>
         </is>
@@ -473,332 +478,34 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>rs10885502</t>
+          <t>193    rs72826020
+Name: ID, dtype: object</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>WAS</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2.98794 (1.30006, 6.86721)</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0.00993727</v>
-      </c>
-      <c r="F2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>HC1007_TTE_acute_upper_respiratory_infections_of_multiple_and_unspecified_sites</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>rs295271</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
           <t>EUR</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1.0266 (1.01182, 1.0416)</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0.000388439</v>
-      </c>
-      <c r="F3" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>HC643_TTE_other_hypothyroidism</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>rs2256183</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>WAS</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>34.5599 (2.70267, 441.929)</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0.00643766</v>
-      </c>
-      <c r="F4" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>HC1581_AD_asthma</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>rs9268832</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0.796965 (0.727965, 0.872504)</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>9.02185e-07</v>
-      </c>
-      <c r="F5" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>HC221_Diabetes</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>rs8192653</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>1.06191 (1.02214, 1.10323)</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>0.00204024</v>
-      </c>
-      <c r="F6" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>HC382_Asthma</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>rs2855812</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>1.09698 (1.07604, 1.11832)</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>4.7038e-21</v>
-      </c>
-      <c r="F7" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>HC1581_AD_asthma</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>rs2855812</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>1.09712 (1.07606, 1.1186)</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>7.09846e-21</v>
-      </c>
-      <c r="F8" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>HC219_Hypothyroidism/myxoedema</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>rs2256183</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>WAS</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>34.5599 (2.70267, 441.929)</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>0.00643766</v>
-      </c>
-      <c r="F9" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>HC382_Asthma</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>rs9268832</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>0.798201 (0.729279, 0.873636)</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>9.98182e-07</v>
-      </c>
-      <c r="F10" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>FH1220_Diabetes_(FH)</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>rs61741902</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>0.642298 (0.485983, 0.848891)</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>0.00186249</v>
-      </c>
-      <c r="F11" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>HC1036_TTE_asthma</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>rs9268832</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>0.802466 (0.733554, 0.877852)</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>1.55726e-06</v>
-      </c>
-      <c r="F12" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>HC221_Diabetes</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>rs77657273</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>1.07479 (1.02462, 1.12741)</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>0.00310343</v>
-      </c>
-      <c r="F13" t="n">
-        <v>14</v>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>193    0.89809
+Name: OR, dtype: float64 (193    0.840833
+Name: L95, dtype: float64, 193    0.959245
+Name: U95, dtype: float64)</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>193    0.001384
+Name: P, dtype: float64</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>&lt;built-in function chr&gt;</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>